<commit_message>
phillip du skal have en omgang med spanskrøret
</commit_message>
<xml_diff>
--- a/Date_State_Observation.xlsx
+++ b/Date_State_Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Desktop\UNI\DataVisualization\R_opgaver\Project\DataVis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCB6EC-CD74-44D9-BBBC-517262C1A39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B72EC-DE4A-4026-9A29-D9F6E27E880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A969E9E3-D461-4946-9C5A-00A3E51BC3F2}"/>
   </bookViews>
@@ -1968,7 +1968,7 @@
   <dimension ref="A1:E3776"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>